<commit_message>
changed tt_simulation.xlsx for better score calculation
</commit_message>
<xml_diff>
--- a/supporting_info/tt_simulation.xlsx
+++ b/supporting_info/tt_simulation.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Desktop\New_folder\TTMS\supporting_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8343226B-75B7-4ADF-996D-6A05DE55C9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B0F41F-336F-444B-BFE2-BEEC6DF6BAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="13812" windowHeight="8664" xr2:uid="{3E355DBB-BB44-42DC-BF0C-E072063C6D9E}"/>
+    <workbookView xWindow="4692" yWindow="0" windowWidth="15564" windowHeight="12360" xr2:uid="{3E355DBB-BB44-42DC-BF0C-E072063C6D9E}"/>
   </bookViews>
   <sheets>
     <sheet name="tt_simulation_1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Player</t>
   </si>
@@ -68,9 +69,6 @@
     <t>P11</t>
   </si>
   <si>
-    <t>max ave points</t>
-  </si>
-  <si>
     <t>P01</t>
   </si>
   <si>
@@ -96,6 +94,21 @@
   </si>
   <si>
     <t>P09</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>winner_average</t>
+  </si>
+  <si>
+    <t>loser_average</t>
+  </si>
+  <si>
+    <t>max total points</t>
   </si>
 </sst>
 </file>
@@ -600,7 +613,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -610,6 +623,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -658,74 +674,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -742,10 +690,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="5C5C5C"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -1054,15 +1002,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C98B65B-A82E-4150-8791-00327E6EE058}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1088,9 +1036,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2">
         <v>6</v>
@@ -1099,6 +1047,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2">
+        <f>5-C2</f>
         <v>0</v>
       </c>
       <c r="E2" s="2">
@@ -1108,17 +1057,21 @@
         <v>0.73</v>
       </c>
       <c r="G2" s="2">
-        <f>E2*F2</f>
-        <v>3.65</v>
+        <f>E2+C2*F2</f>
+        <v>8.65</v>
       </c>
       <c r="H2" s="2">
         <f>IF(12-ROUND(12*(G2/$H$16),1)=0,1,12-ROUND(12*(G2/$H$16),1))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.5999999999999996</v>
+      </c>
+      <c r="I2" s="2">
+        <f>12-ROUND(12*(G2/$H$16),1)</f>
+        <v>1.5999999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2">
         <v>6</v>
@@ -1127,6 +1080,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="2">
+        <f t="shared" ref="D3:D13" si="0">5-C3</f>
         <v>1</v>
       </c>
       <c r="E3" s="2">
@@ -1136,17 +1090,21 @@
         <v>0.91</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G13" si="0">E3*F3</f>
-        <v>3.64</v>
+        <f>E3+C3*F3</f>
+        <v>7.6400000000000006</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" ref="H3:H13" si="1">IF(12-ROUND(12*(G3/$H$16),1)=0,1,12-ROUND(12*(G3/$H$16),1))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2.8000000000000007</v>
+      </c>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I13" si="2">12-ROUND(12*(G3/$H$16),1)</f>
+        <v>2.8000000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -1155,6 +1113,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="2">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E4" s="2">
@@ -1164,15 +1123,19 @@
         <v>0.91</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" si="0"/>
-        <v>3.64</v>
+        <f t="shared" ref="G3:G13" si="3">E4+C4*F4</f>
+        <v>7.6400000000000006</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2.8000000000000007</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" si="2"/>
+        <v>2.8000000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1183,6 +1146,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="2">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E5" s="2">
@@ -1192,15 +1156,19 @@
         <v>0.73</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>2.92</v>
+        <f t="shared" si="3"/>
+        <v>6.92</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="1"/>
-        <v>2.4000000000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>3.6999999999999993</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="2"/>
+        <v>3.6999999999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1211,6 +1179,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="2">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E6" s="2">
@@ -1220,17 +1189,21 @@
         <v>0.64</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>2.56</v>
+        <f t="shared" si="3"/>
+        <v>6.5600000000000005</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" si="1"/>
-        <v>3.5999999999999996</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="2"/>
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -1239,6 +1212,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="2">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E7" s="2">
@@ -1248,17 +1222,21 @@
         <v>0.36</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>1.08</v>
+        <f t="shared" si="3"/>
+        <v>4.08</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="1"/>
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>7.1</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="2"/>
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2">
         <v>6</v>
@@ -1267,6 +1245,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="2">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E8" s="2">
@@ -1276,17 +1255,21 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
+        <f t="shared" si="3"/>
+        <v>3.1</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="1"/>
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="2"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
         <v>9</v>
@@ -1295,6 +1278,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="2">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E9" s="2">
@@ -1304,15 +1288,19 @@
         <v>0.64</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>0.64</v>
+        <f t="shared" si="3"/>
+        <v>1.6400000000000001</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" si="1"/>
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1323,6 +1311,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="2">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E10" s="2">
@@ -1332,17 +1321,21 @@
         <v>0.45</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0.45</v>
+        <f t="shared" si="3"/>
+        <v>1.45</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="1"/>
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>10.3</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="2"/>
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>9</v>
@@ -1351,6 +1344,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="2">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E11" s="2">
@@ -1360,17 +1354,21 @@
         <v>0.18</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0.36</v>
+        <f t="shared" si="3"/>
+        <v>2.36</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="1"/>
-        <v>10.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <f>IF(12-ROUND(12*(G11/$H$16),1)=0,1,12-ROUND(12*(G11/$H$16),1))</f>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="2"/>
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2">
         <v>9</v>
@@ -1379,6 +1377,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="2">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E12" s="2">
@@ -1388,17 +1387,21 @@
         <v>0</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2">
         <v>9</v>
@@ -1407,6 +1410,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="2">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E13" s="2">
@@ -1416,27 +1420,156 @@
         <v>0</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G16" t="s">
-        <v>11</v>
-      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="4"/>
       <c r="H16">
-        <f>MAX(G2:G13)</f>
-        <v>3.65</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H13">
     <sortCondition ref="H1:H13"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="F16:G16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8CBB72-6F91-49B3-935E-F0B211D11522}">
+  <dimension ref="A2:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <f>ABS(B2-A2)/11</f>
+        <v>0.54545454545454541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D6" si="0">ABS(B3-A3)/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.18181818181818182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.27272727272727271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.18181818181818182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <f>AVERAGEIF(C2:C6,"w",D2:D6)</f>
+        <v>0.30303030303030304</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <f>D8*3+E8</f>
+        <v>3.9090909090909092</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <f>AVERAGEIF(C3:C7,"l",D3:D7)</f>
+        <v>0.22727272727272727</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <f>D9*2+E9</f>
+        <v>2.4545454545454546</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>